<commit_message>
'added card printer elem'
</commit_message>
<xml_diff>
--- a/ecard-infos.xlsx
+++ b/ecard-infos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Class-Infos" sheetId="1" state="visible" r:id="rId2"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="248">
   <si>
     <t xml:space="preserve">Adviser’s Name </t>
   </si>
@@ -466,9 +466,6 @@
   </si>
   <si>
     <t xml:space="preserve">JURIELYN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VILLAGANAS</t>
   </si>
   <si>
     <t xml:space="preserve">BAGUIO</t>
@@ -962,8 +959,8 @@
   </sheetPr>
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="M13:N13 B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E77" activeCellId="0" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1552,6 +1549,16 @@
         <v>16</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>24</v>
@@ -2219,9 +2226,6 @@
       <c r="D71" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="F71" s="2" t="str">
         <f aca="false">IF(ISBLANK(C71), "", "FEMALE")</f>
         <v>FEMALE</v>
@@ -2238,13 +2242,13 @@
         <v>136514120100</v>
       </c>
       <c r="C72" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="E72" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="E72" s="0" t="s">
-        <v>141</v>
       </c>
       <c r="F72" s="2" t="str">
         <f aca="false">IF(ISBLANK(C72), "", "FEMALE")</f>
@@ -2262,13 +2266,13 @@
         <v>106499130010</v>
       </c>
       <c r="C73" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D73" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="E73" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="E73" s="0" t="s">
-        <v>144</v>
       </c>
       <c r="F73" s="2" t="str">
         <f aca="false">IF(ISBLANK(C73), "", "FEMALE")</f>
@@ -2286,13 +2290,13 @@
         <v>136829110055</v>
       </c>
       <c r="C74" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D74" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="E74" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="E74" s="0" t="s">
-        <v>147</v>
       </c>
       <c r="F74" s="2" t="str">
         <f aca="false">IF(ISBLANK(C74), "", "FEMALE")</f>
@@ -2465,7 +2469,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="M13:N13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2477,46 +2481,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>202</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +2942,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="M13:N13 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2950,46 +2954,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,7 +3203,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,7 +3415,7 @@
   <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X3" activeCellId="1" sqref="M13:N13 X3"/>
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3450,94 +3454,94 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3957,11 +3961,11 @@
       </c>
       <c r="M5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M5="", "", VLOOKUP('Compute-Values-Male'!M5, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N5="", "", VLOOKUP('Compute-Values-Male'!N5, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="O5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O5="", "", VLOOKUP('Compute-Values-Male'!O5, values_lookup, 3, 1))</f>
@@ -3969,7 +3973,7 @@
       </c>
       <c r="P5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!P5="", "", VLOOKUP('Compute-Values-Male'!P5, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="Q5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!Q5="", "", VLOOKUP('Compute-Values-Male'!Q5, values_lookup, 3, 1))</f>
@@ -3977,27 +3981,27 @@
       </c>
       <c r="R5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!R5="", "", VLOOKUP('Compute-Values-Male'!R5, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="S5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!S5="", "", VLOOKUP('Compute-Values-Male'!S5, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T5="", "", VLOOKUP('Compute-Values-Male'!T5, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U5="", "", VLOOKUP('Compute-Values-Male'!U5, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="V5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V5="", "", VLOOKUP('Compute-Values-Male'!V5, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W5="", "", VLOOKUP('Compute-Values-Male'!W5, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X5" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X5="", "", VLOOKUP('Compute-Values-Male'!X5, values_lookup, 3, 1))</f>
@@ -4161,7 +4165,7 @@
       </c>
       <c r="C7" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!C7="", "", VLOOKUP('Compute-Values-Male'!C7, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D7" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!D7="", "", VLOOKUP('Compute-Values-Male'!D7, values_lookup, 3, 1))</f>
@@ -4201,11 +4205,11 @@
       </c>
       <c r="M7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M7="", "", VLOOKUP('Compute-Values-Male'!M7, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N7="", "", VLOOKUP('Compute-Values-Male'!N7, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="O7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O7="", "", VLOOKUP('Compute-Values-Male'!O7, values_lookup, 3, 1))</f>
@@ -4229,19 +4233,19 @@
       </c>
       <c r="T7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T7="", "", VLOOKUP('Compute-Values-Male'!T7, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U7="", "", VLOOKUP('Compute-Values-Male'!U7, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="V7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V7="", "", VLOOKUP('Compute-Values-Male'!V7, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W7="", "", VLOOKUP('Compute-Values-Male'!W7, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X7" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X7="", "", VLOOKUP('Compute-Values-Male'!X7, values_lookup, 3, 1))</f>
@@ -4323,11 +4327,11 @@
       </c>
       <c r="M8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M8="", "", VLOOKUP('Compute-Values-Male'!M8, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N8="", "", VLOOKUP('Compute-Values-Male'!N8, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="O8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O8="", "", VLOOKUP('Compute-Values-Male'!O8, values_lookup, 3, 1))</f>
@@ -4351,19 +4355,19 @@
       </c>
       <c r="T8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T8="", "", VLOOKUP('Compute-Values-Male'!T8, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U8="", "", VLOOKUP('Compute-Values-Male'!U8, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="V8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V8="", "", VLOOKUP('Compute-Values-Male'!V8, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W8="", "", VLOOKUP('Compute-Values-Male'!W8, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X8" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X8="", "", VLOOKUP('Compute-Values-Male'!X8, values_lookup, 3, 1))</f>
@@ -4567,11 +4571,11 @@
       </c>
       <c r="M10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M10="", "", VLOOKUP('Compute-Values-Male'!M10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N10="", "", VLOOKUP('Compute-Values-Male'!N10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="O10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O10="", "", VLOOKUP('Compute-Values-Male'!O10, values_lookup, 3, 1))</f>
@@ -4595,19 +4599,19 @@
       </c>
       <c r="T10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T10="", "", VLOOKUP('Compute-Values-Male'!T10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U10="", "", VLOOKUP('Compute-Values-Male'!U10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="V10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V10="", "", VLOOKUP('Compute-Values-Male'!V10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>SO</v>
       </c>
       <c r="W10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W10="", "", VLOOKUP('Compute-Values-Male'!W10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X10="", "", VLOOKUP('Compute-Values-Male'!X10, values_lookup, 3, 1))</f>
@@ -4665,7 +4669,7 @@
       </c>
       <c r="G11" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!G11="", "", VLOOKUP('Compute-Values-Male'!G11, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H11" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!H11="", "", VLOOKUP('Compute-Values-Male'!H11, values_lookup, 3, 1))</f>
@@ -4689,11 +4693,11 @@
       </c>
       <c r="M11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M11="", "", VLOOKUP('Compute-Values-Male'!M11, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N11="", "", VLOOKUP('Compute-Values-Male'!N11, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="O11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O11="", "", VLOOKUP('Compute-Values-Male'!O11, values_lookup, 3, 1))</f>
@@ -4717,11 +4721,11 @@
       </c>
       <c r="T11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T11="", "", VLOOKUP('Compute-Values-Male'!T11, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U11="", "", VLOOKUP('Compute-Values-Male'!U11, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V11="", "", VLOOKUP('Compute-Values-Male'!V11, values_lookup, 3, 1))</f>
@@ -4729,7 +4733,7 @@
       </c>
       <c r="W11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W11="", "", VLOOKUP('Compute-Values-Male'!W11, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X11" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X11="", "", VLOOKUP('Compute-Values-Male'!X11, values_lookup, 3, 1))</f>
@@ -4949,7 +4953,7 @@
       </c>
       <c r="Q13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!Q13="", "", VLOOKUP('Compute-Values-Male'!Q13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="R13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!R13="", "", VLOOKUP('Compute-Values-Male'!R13, values_lookup, 3, 1))</f>
@@ -4973,7 +4977,7 @@
       </c>
       <c r="W13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W13="", "", VLOOKUP('Compute-Values-Male'!W13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X13="", "", VLOOKUP('Compute-Values-Male'!X13, values_lookup, 3, 1))</f>
@@ -5015,7 +5019,7 @@
       </c>
       <c r="C14" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!C14="", "", VLOOKUP('Compute-Values-Male'!C14, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D14" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!D14="", "", VLOOKUP('Compute-Values-Male'!D14, values_lookup, 3, 1))</f>
@@ -5641,7 +5645,7 @@
       </c>
       <c r="G19" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!G19="", "", VLOOKUP('Compute-Values-Male'!G19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H19" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!H19="", "", VLOOKUP('Compute-Values-Male'!H19, values_lookup, 3, 1))</f>
@@ -5665,15 +5669,15 @@
       </c>
       <c r="M19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!M19="", "", VLOOKUP('Compute-Values-Male'!M19, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!N19="", "", VLOOKUP('Compute-Values-Male'!N19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="O19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!O19="", "", VLOOKUP('Compute-Values-Male'!O19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="P19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!P19="", "", VLOOKUP('Compute-Values-Male'!P19, values_lookup, 3, 1))</f>
@@ -5681,7 +5685,7 @@
       </c>
       <c r="Q19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!Q19="", "", VLOOKUP('Compute-Values-Male'!Q19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="R19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!R19="", "", VLOOKUP('Compute-Values-Male'!R19, values_lookup, 3, 1))</f>
@@ -5697,7 +5701,7 @@
       </c>
       <c r="U19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U19="", "", VLOOKUP('Compute-Values-Male'!U19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V19="", "", VLOOKUP('Compute-Values-Male'!V19, values_lookup, 3, 1))</f>
@@ -5705,7 +5709,7 @@
       </c>
       <c r="W19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W19="", "", VLOOKUP('Compute-Values-Male'!W19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X19="", "", VLOOKUP('Compute-Values-Male'!X19, values_lookup, 3, 1))</f>
@@ -5763,7 +5767,7 @@
       </c>
       <c r="G20" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!G20="", "", VLOOKUP('Compute-Values-Male'!G20, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H20" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!H20="", "", VLOOKUP('Compute-Values-Male'!H20, values_lookup, 3, 1))</f>
@@ -5815,19 +5819,19 @@
       </c>
       <c r="T20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T20="", "", VLOOKUP('Compute-Values-Male'!T20, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U20="", "", VLOOKUP('Compute-Values-Male'!U20, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="V20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V20="", "", VLOOKUP('Compute-Values-Male'!V20, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W20="", "", VLOOKUP('Compute-Values-Male'!W20, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X20="", "", VLOOKUP('Compute-Values-Male'!X20, values_lookup, 3, 1))</f>
@@ -5881,11 +5885,11 @@
       </c>
       <c r="F21" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!F21="", "", VLOOKUP('Compute-Values-Male'!F21, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="G21" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!G21="", "", VLOOKUP('Compute-Values-Male'!G21, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H21" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!H21="", "", VLOOKUP('Compute-Values-Male'!H21, values_lookup, 3, 1))</f>
@@ -5937,11 +5941,11 @@
       </c>
       <c r="T21" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T21="", "", VLOOKUP('Compute-Values-Male'!T21, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U21" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U21="", "", VLOOKUP('Compute-Values-Male'!U21, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V21" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V21="", "", VLOOKUP('Compute-Values-Male'!V21, values_lookup, 3, 1))</f>
@@ -5949,7 +5953,7 @@
       </c>
       <c r="W21" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!W21="", "", VLOOKUP('Compute-Values-Male'!W21, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X21" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!X21="", "", VLOOKUP('Compute-Values-Male'!X21, values_lookup, 3, 1))</f>
@@ -5991,7 +5995,7 @@
       </c>
       <c r="C22" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!C22="", "", VLOOKUP('Compute-Values-Male'!C22, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="D22" s="8" t="str">
         <f aca="false">IF('Compute-Values-Male'!D22="", "", VLOOKUP('Compute-Values-Male'!D22, values_lookup, 3, 1))</f>
@@ -6059,11 +6063,11 @@
       </c>
       <c r="T22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!T22="", "", VLOOKUP('Compute-Values-Male'!T22, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>SO</v>
       </c>
       <c r="U22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!U22="", "", VLOOKUP('Compute-Values-Male'!U22, values_lookup, 3, 1))</f>
-        <v/>
+        <v>AO</v>
       </c>
       <c r="V22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Male'!V22="", "", VLOOKUP('Compute-Values-Male'!V22, values_lookup, 3, 1))</f>
@@ -8439,7 +8443,7 @@
   <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE30" activeCellId="1" sqref="M13:N13 AE30"/>
+      <selection pane="topLeft" activeCell="AE30" activeCellId="0" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8478,94 +8482,94 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8835,11 +8839,11 @@
       </c>
       <c r="F4" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!F4="", "", VLOOKUP('Compute-Values-Female'!F4, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="G4" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G4="", "", VLOOKUP('Compute-Values-Female'!G4, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="H4" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H4="", "", VLOOKUP('Compute-Values-Female'!H4, values_lookup, 3, 1))</f>
@@ -9433,7 +9437,7 @@
       </c>
       <c r="C9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C9="", "", VLOOKUP('Compute-Values-Female'!C9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D9="", "", VLOOKUP('Compute-Values-Female'!D9, values_lookup, 3, 1))</f>
@@ -9449,7 +9453,7 @@
       </c>
       <c r="G9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G9="", "", VLOOKUP('Compute-Values-Female'!G9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H9="", "", VLOOKUP('Compute-Values-Female'!H9, values_lookup, 3, 1))</f>
@@ -9457,7 +9461,7 @@
       </c>
       <c r="I9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!I9="", "", VLOOKUP('Compute-Values-Female'!I9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="J9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!J9="", "", VLOOKUP('Compute-Values-Female'!J9, values_lookup, 3, 1))</f>
@@ -9465,11 +9469,11 @@
       </c>
       <c r="K9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!K9="", "", VLOOKUP('Compute-Values-Female'!K9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="L9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!L9="", "", VLOOKUP('Compute-Values-Female'!L9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="M9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M9="", "", VLOOKUP('Compute-Values-Female'!M9, values_lookup, 3, 1))</f>
@@ -9477,35 +9481,35 @@
       </c>
       <c r="N9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N9="", "", VLOOKUP('Compute-Values-Female'!N9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="O9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!O9="", "", VLOOKUP('Compute-Values-Female'!O9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="P9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!P9="", "", VLOOKUP('Compute-Values-Female'!P9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="Q9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!Q9="", "", VLOOKUP('Compute-Values-Female'!Q9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="R9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!R9="", "", VLOOKUP('Compute-Values-Female'!R9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="S9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S9="", "", VLOOKUP('Compute-Values-Female'!S9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T9="", "", VLOOKUP('Compute-Values-Female'!T9, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U9="", "", VLOOKUP('Compute-Values-Female'!U9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V9="", "", VLOOKUP('Compute-Values-Female'!V9, values_lookup, 3, 1))</f>
@@ -9513,7 +9517,7 @@
       </c>
       <c r="W9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!W9="", "", VLOOKUP('Compute-Values-Female'!W9, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X9" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!X9="", "", VLOOKUP('Compute-Values-Female'!X9, values_lookup, 3, 1))</f>
@@ -9555,11 +9559,11 @@
       </c>
       <c r="C10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C10="", "", VLOOKUP('Compute-Values-Female'!C10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D10="", "", VLOOKUP('Compute-Values-Female'!D10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="E10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!E10="", "", VLOOKUP('Compute-Values-Female'!E10, values_lookup, 3, 1))</f>
@@ -9567,11 +9571,11 @@
       </c>
       <c r="F10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!F10="", "", VLOOKUP('Compute-Values-Female'!F10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="G10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G10="", "", VLOOKUP('Compute-Values-Female'!G10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H10="", "", VLOOKUP('Compute-Values-Female'!H10, values_lookup, 3, 1))</f>
@@ -9587,23 +9591,23 @@
       </c>
       <c r="K10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!K10="", "", VLOOKUP('Compute-Values-Female'!K10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="L10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!L10="", "", VLOOKUP('Compute-Values-Female'!L10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="M10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M10="", "", VLOOKUP('Compute-Values-Female'!M10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N10="", "", VLOOKUP('Compute-Values-Female'!N10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="O10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!O10="", "", VLOOKUP('Compute-Values-Female'!O10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="P10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!P10="", "", VLOOKUP('Compute-Values-Female'!P10, values_lookup, 3, 1))</f>
@@ -9615,19 +9619,19 @@
       </c>
       <c r="R10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!R10="", "", VLOOKUP('Compute-Values-Female'!R10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="S10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S10="", "", VLOOKUP('Compute-Values-Female'!S10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T10="", "", VLOOKUP('Compute-Values-Female'!T10, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U10="", "", VLOOKUP('Compute-Values-Female'!U10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V10="", "", VLOOKUP('Compute-Values-Female'!V10, values_lookup, 3, 1))</f>
@@ -9635,7 +9639,7 @@
       </c>
       <c r="W10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!W10="", "", VLOOKUP('Compute-Values-Female'!W10, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X10" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!X10="", "", VLOOKUP('Compute-Values-Female'!X10, values_lookup, 3, 1))</f>
@@ -9839,11 +9843,11 @@
       </c>
       <c r="M12" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M12="", "", VLOOKUP('Compute-Values-Female'!M12, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>SO</v>
       </c>
       <c r="N12" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N12="", "", VLOOKUP('Compute-Values-Female'!N12, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="O12" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!O12="", "", VLOOKUP('Compute-Values-Female'!O12, values_lookup, 3, 1))</f>
@@ -9921,7 +9925,7 @@
       </c>
       <c r="C13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C13="", "", VLOOKUP('Compute-Values-Female'!C13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="D13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D13="", "", VLOOKUP('Compute-Values-Female'!D13, values_lookup, 3, 1))</f>
@@ -9933,11 +9937,11 @@
       </c>
       <c r="F13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!F13="", "", VLOOKUP('Compute-Values-Female'!F13, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="G13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G13="", "", VLOOKUP('Compute-Values-Female'!G13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H13="", "", VLOOKUP('Compute-Values-Female'!H13, values_lookup, 3, 1))</f>
@@ -9961,15 +9965,15 @@
       </c>
       <c r="M13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M13="", "", VLOOKUP('Compute-Values-Female'!M13, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N13="", "", VLOOKUP('Compute-Values-Female'!N13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="O13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!O13="", "", VLOOKUP('Compute-Values-Female'!O13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="P13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!P13="", "", VLOOKUP('Compute-Values-Female'!P13, values_lookup, 3, 1))</f>
@@ -9985,7 +9989,7 @@
       </c>
       <c r="S13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S13="", "", VLOOKUP('Compute-Values-Female'!S13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T13="", "", VLOOKUP('Compute-Values-Female'!T13, values_lookup, 3, 1))</f>
@@ -9993,7 +9997,7 @@
       </c>
       <c r="U13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U13="", "", VLOOKUP('Compute-Values-Female'!U13, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="V13" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V13="", "", VLOOKUP('Compute-Values-Female'!V13, values_lookup, 3, 1))</f>
@@ -10233,19 +10237,19 @@
       </c>
       <c r="T15" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T15="", "", VLOOKUP('Compute-Values-Female'!T15, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U15" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U15="", "", VLOOKUP('Compute-Values-Female'!U15, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="V15" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V15="", "", VLOOKUP('Compute-Values-Female'!V15, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W15" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!W15="", "", VLOOKUP('Compute-Values-Female'!W15, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X15" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!X15="", "", VLOOKUP('Compute-Values-Female'!X15, values_lookup, 3, 1))</f>
@@ -10287,7 +10291,7 @@
       </c>
       <c r="C16" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C16="", "", VLOOKUP('Compute-Values-Female'!C16, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="D16" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D16="", "", VLOOKUP('Compute-Values-Female'!D16, values_lookup, 3, 1))</f>
@@ -10355,11 +10359,11 @@
       </c>
       <c r="T16" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T16="", "", VLOOKUP('Compute-Values-Female'!T16, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="U16" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U16="", "", VLOOKUP('Compute-Values-Female'!U16, values_lookup, 3, 1))</f>
-        <v/>
+        <v>SO</v>
       </c>
       <c r="V16" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V16="", "", VLOOKUP('Compute-Values-Female'!V16, values_lookup, 3, 1))</f>
@@ -10543,11 +10547,11 @@
       </c>
       <c r="F18" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!F18="", "", VLOOKUP('Compute-Values-Female'!F18, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="G18" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G18="", "", VLOOKUP('Compute-Values-Female'!G18, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="H18" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H18="", "", VLOOKUP('Compute-Values-Female'!H18, values_lookup, 3, 1))</f>
@@ -10653,7 +10657,7 @@
       </c>
       <c r="C19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C19="", "", VLOOKUP('Compute-Values-Female'!C19, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D19" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D19="", "", VLOOKUP('Compute-Values-Female'!D19, values_lookup, 3, 1))</f>
@@ -10807,7 +10811,7 @@
       </c>
       <c r="K20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!K20="", "", VLOOKUP('Compute-Values-Female'!K20, values_lookup, 3, 1))</f>
-        <v>SO</v>
+        <v>AO</v>
       </c>
       <c r="L20" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!L20="", "", VLOOKUP('Compute-Values-Female'!L20, values_lookup, 3, 1))</f>
@@ -11015,7 +11019,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C22="", "", VLOOKUP('Compute-Values-Female'!C22, values_lookup, 3, 1))</f>
@@ -11079,11 +11083,11 @@
       </c>
       <c r="R22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!R22="", "", VLOOKUP('Compute-Values-Female'!R22, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="S22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S22="", "", VLOOKUP('Compute-Values-Female'!S22, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T22" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T22="", "", VLOOKUP('Compute-Values-Female'!T22, values_lookup, 3, 1))</f>
@@ -11173,7 +11177,7 @@
       </c>
       <c r="K23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!K23="", "", VLOOKUP('Compute-Values-Female'!K23, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="L23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!L23="", "", VLOOKUP('Compute-Values-Female'!L23, values_lookup, 3, 1))</f>
@@ -11181,11 +11185,11 @@
       </c>
       <c r="M23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M23="", "", VLOOKUP('Compute-Values-Female'!M23, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="N23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N23="", "", VLOOKUP('Compute-Values-Female'!N23, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="O23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!O23="", "", VLOOKUP('Compute-Values-Female'!O23, values_lookup, 3, 1))</f>
@@ -11201,11 +11205,11 @@
       </c>
       <c r="R23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!R23="", "", VLOOKUP('Compute-Values-Female'!R23, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="S23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S23="", "", VLOOKUP('Compute-Values-Female'!S23, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T23="", "", VLOOKUP('Compute-Values-Female'!T23, values_lookup, 3, 1))</f>
@@ -11213,7 +11217,7 @@
       </c>
       <c r="U23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U23="", "", VLOOKUP('Compute-Values-Female'!U23, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="V23" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V23="", "", VLOOKUP('Compute-Values-Female'!V23, values_lookup, 3, 1))</f>
@@ -11385,11 +11389,11 @@
       </c>
       <c r="C25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!C25="", "", VLOOKUP('Compute-Values-Female'!C25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="D25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!D25="", "", VLOOKUP('Compute-Values-Female'!D25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="E25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!E25="", "", VLOOKUP('Compute-Values-Female'!E25, values_lookup, 3, 1))</f>
@@ -11397,11 +11401,11 @@
       </c>
       <c r="F25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!F25="", "", VLOOKUP('Compute-Values-Female'!F25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="G25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!G25="", "", VLOOKUP('Compute-Values-Female'!G25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="H25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!H25="", "", VLOOKUP('Compute-Values-Female'!H25, values_lookup, 3, 1))</f>
@@ -11425,7 +11429,7 @@
       </c>
       <c r="M25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!M25="", "", VLOOKUP('Compute-Values-Female'!M25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="N25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!N25="", "", VLOOKUP('Compute-Values-Female'!N25, values_lookup, 3, 1))</f>
@@ -11449,7 +11453,7 @@
       </c>
       <c r="S25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!S25="", "", VLOOKUP('Compute-Values-Female'!S25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="T25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!T25="", "", VLOOKUP('Compute-Values-Female'!T25, values_lookup, 3, 1))</f>
@@ -11457,15 +11461,15 @@
       </c>
       <c r="U25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!U25="", "", VLOOKUP('Compute-Values-Female'!U25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>RO</v>
       </c>
       <c r="V25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!V25="", "", VLOOKUP('Compute-Values-Female'!V25, values_lookup, 3, 1))</f>
-        <v>NO</v>
+        <v>RO</v>
       </c>
       <c r="W25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!W25="", "", VLOOKUP('Compute-Values-Female'!W25, values_lookup, 3, 1))</f>
-        <v/>
+        <v>NO</v>
       </c>
       <c r="X25" s="9" t="str">
         <f aca="false">IF('Compute-Values-Female'!X25="", "", VLOOKUP('Compute-Values-Female'!X25, values_lookup, 3, 1))</f>
@@ -13467,7 +13471,7 @@
   <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="M13:N13 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13506,48 +13510,48 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14338,7 +14342,7 @@
   <dimension ref="A1:AD42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="M13:N13 C1"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14377,48 +14381,48 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14948,7 +14952,7 @@
       </c>
       <c r="B23" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
@@ -15228,7 +15232,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="W1" activeCellId="0" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="X28" activeCellId="1" sqref="M13:N13 X28"/>
+      <selection pane="bottomRight" activeCell="X28" activeCellId="0" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15267,94 +15271,94 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15774,11 +15778,11 @@
       </c>
       <c r="M5" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F5="", "", ROUND(('2nd-Summary-Male'!F5+'2nd-Summary-Male'!G5)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="N5" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="N5" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G5="", "", ROUND(('2nd-Summary-Male'!G5+'2nd-Summary-Male'!H5)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="O5" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H5="", "", ROUND(('2nd-Summary-Male'!H5+'2nd-Summary-Male'!I5)/2, 0))</f>
@@ -15786,7 +15790,7 @@
       </c>
       <c r="P5" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!I5="", "", ROUND(('2nd-Summary-Male'!I5+'2nd-Summary-Male'!J5)/2, 0))</f>
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!C5="", "", ROUND(('3rd-Summary-Male'!C5+'3rd-Summary-Male'!D5)/2, 0))</f>
@@ -15794,27 +15798,27 @@
       </c>
       <c r="R5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!D5="", "", ROUND(('3rd-Summary-Male'!D5+'3rd-Summary-Male'!E5)/2, 0))</f>
-        <v>40</v>
-      </c>
-      <c r="S5" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="S5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!E5="", "", ROUND(('3rd-Summary-Male'!E5+'3rd-Summary-Male'!F5)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="T5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F5="", "", ROUND(('3rd-Summary-Male'!F5+'3rd-Summary-Male'!G5)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U5" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G5="", "", ROUND(('3rd-Summary-Male'!G5+'3rd-Summary-Male'!H5)/2, 0))</f>
-        <v/>
+        <v>80</v>
       </c>
       <c r="V5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H5="", "", ROUND(('3rd-Summary-Male'!H5+'3rd-Summary-Male'!I5)/2, 0))</f>
-        <v>42</v>
-      </c>
-      <c r="W5" s="9" t="str">
+        <v>79</v>
+      </c>
+      <c r="W5" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I5="", "", ROUND(('3rd-Summary-Male'!I5+'3rd-Summary-Male'!J5)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X5" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C5="", "", ROUND(('4th-Summary-Male'!C5+'4th-Summary-Male'!D5)/2, 0))</f>
@@ -15976,9 +15980,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C15), "", CONCATENATE('Class-Infos'!C15, ", ", 'Class-Infos'!D15, " ", 'Class-Infos'!E15))</f>
         <v>ALEJANDRO, MARK AGBUYA</v>
       </c>
-      <c r="C7" s="8" t="str">
+      <c r="C7" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!C7="", "", ROUND(('1st-Summary-Male'!C7+'1st-Summary-Male'!D7)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="D7" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!D7="", "", ROUND(('1st-Summary-Male'!D7+'1st-Summary-Male'!E7)/2, 0))</f>
@@ -16018,11 +16022,11 @@
       </c>
       <c r="M7" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F7="", "", ROUND(('2nd-Summary-Male'!F7+'2nd-Summary-Male'!G7)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="N7" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="N7" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G7="", "", ROUND(('2nd-Summary-Male'!G7+'2nd-Summary-Male'!H7)/2, 0))</f>
-        <v/>
+        <v>78</v>
       </c>
       <c r="O7" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H7="", "", ROUND(('2nd-Summary-Male'!H7+'2nd-Summary-Male'!I7)/2, 0))</f>
@@ -16030,7 +16034,7 @@
       </c>
       <c r="P7" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!I7="", "", ROUND(('2nd-Summary-Male'!I7+'2nd-Summary-Male'!J7)/2, 0))</f>
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="Q7" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!C7="", "", ROUND(('3rd-Summary-Male'!C7+'3rd-Summary-Male'!D7)/2, 0))</f>
@@ -16046,19 +16050,19 @@
       </c>
       <c r="T7" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F7="", "", ROUND(('3rd-Summary-Male'!F7+'3rd-Summary-Male'!G7)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U7" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U7" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G7="", "", ROUND(('3rd-Summary-Male'!G7+'3rd-Summary-Male'!H7)/2, 0))</f>
-        <v/>
+        <v>80</v>
       </c>
       <c r="V7" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H7="", "", ROUND(('3rd-Summary-Male'!H7+'3rd-Summary-Male'!I7)/2, 0))</f>
-        <v>42</v>
-      </c>
-      <c r="W7" s="9" t="str">
+        <v>80</v>
+      </c>
+      <c r="W7" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I7="", "", ROUND(('3rd-Summary-Male'!I7+'3rd-Summary-Male'!J7)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X7" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C7="", "", ROUND(('4th-Summary-Male'!C7+'4th-Summary-Male'!D7)/2, 0))</f>
@@ -16140,11 +16144,11 @@
       </c>
       <c r="M8" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F8="", "", ROUND(('2nd-Summary-Male'!F8+'2nd-Summary-Male'!G8)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="N8" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="N8" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G8="", "", ROUND(('2nd-Summary-Male'!G8+'2nd-Summary-Male'!H8)/2, 0))</f>
-        <v/>
+        <v>81</v>
       </c>
       <c r="O8" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H8="", "", ROUND(('2nd-Summary-Male'!H8+'2nd-Summary-Male'!I8)/2, 0))</f>
@@ -16168,19 +16172,19 @@
       </c>
       <c r="T8" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F8="", "", ROUND(('3rd-Summary-Male'!F8+'3rd-Summary-Male'!G8)/2, 0))</f>
-        <v>40</v>
-      </c>
-      <c r="U8" s="9" t="str">
+        <v>79</v>
+      </c>
+      <c r="U8" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G8="", "", ROUND(('3rd-Summary-Male'!G8+'3rd-Summary-Male'!H8)/2, 0))</f>
-        <v/>
+        <v>81</v>
       </c>
       <c r="V8" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H8="", "", ROUND(('3rd-Summary-Male'!H8+'3rd-Summary-Male'!I8)/2, 0))</f>
-        <v>42</v>
-      </c>
-      <c r="W8" s="9" t="str">
+        <v>80</v>
+      </c>
+      <c r="W8" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I8="", "", ROUND(('3rd-Summary-Male'!I8+'3rd-Summary-Male'!J8)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X8" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C8="", "", ROUND(('4th-Summary-Male'!C8+'4th-Summary-Male'!D8)/2, 0))</f>
@@ -16384,11 +16388,11 @@
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F10="", "", ROUND(('2nd-Summary-Male'!F10+'2nd-Summary-Male'!G10)/2, 0))</f>
-        <v>40</v>
-      </c>
-      <c r="N10" s="9" t="str">
+        <v>78</v>
+      </c>
+      <c r="N10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G10="", "", ROUND(('2nd-Summary-Male'!G10+'2nd-Summary-Male'!H10)/2, 0))</f>
-        <v/>
+        <v>81</v>
       </c>
       <c r="O10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H10="", "", ROUND(('2nd-Summary-Male'!H10+'2nd-Summary-Male'!I10)/2, 0))</f>
@@ -16412,19 +16416,19 @@
       </c>
       <c r="T10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F10="", "", ROUND(('3rd-Summary-Male'!F10+'3rd-Summary-Male'!G10)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="U10" s="9" t="str">
+        <v>78</v>
+      </c>
+      <c r="U10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G10="", "", ROUND(('3rd-Summary-Male'!G10+'3rd-Summary-Male'!H10)/2, 0))</f>
-        <v/>
+        <v>84</v>
       </c>
       <c r="V10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H10="", "", ROUND(('3rd-Summary-Male'!H10+'3rd-Summary-Male'!I10)/2, 0))</f>
-        <v>45</v>
-      </c>
-      <c r="W10" s="9" t="str">
+        <v>83</v>
+      </c>
+      <c r="W10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I10="", "", ROUND(('3rd-Summary-Male'!I10+'3rd-Summary-Male'!J10)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X10" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C10="", "", ROUND(('4th-Summary-Male'!C10+'4th-Summary-Male'!D10)/2, 0))</f>
@@ -16478,11 +16482,11 @@
       </c>
       <c r="F11" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!F11="", "", ROUND(('1st-Summary-Male'!F11+'1st-Summary-Male'!G11)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="G11" s="8" t="str">
+        <v>75</v>
+      </c>
+      <c r="G11" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!G11="", "", ROUND(('1st-Summary-Male'!G11+'1st-Summary-Male'!H11)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="H11" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!H11="", "", ROUND(('1st-Summary-Male'!H11+'1st-Summary-Male'!I11)/2, 0))</f>
@@ -16506,11 +16510,11 @@
       </c>
       <c r="M11" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F11="", "", ROUND(('2nd-Summary-Male'!F11+'2nd-Summary-Male'!G11)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="N11" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="N11" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G11="", "", ROUND(('2nd-Summary-Male'!G11+'2nd-Summary-Male'!H11)/2, 0))</f>
-        <v/>
+        <v>81</v>
       </c>
       <c r="O11" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H11="", "", ROUND(('2nd-Summary-Male'!H11+'2nd-Summary-Male'!I11)/2, 0))</f>
@@ -16534,19 +16538,19 @@
       </c>
       <c r="T11" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F11="", "", ROUND(('3rd-Summary-Male'!F11+'3rd-Summary-Male'!G11)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U11" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U11" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G11="", "", ROUND(('3rd-Summary-Male'!G11+'3rd-Summary-Male'!H11)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="V11" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H11="", "", ROUND(('3rd-Summary-Male'!H11+'3rd-Summary-Male'!I11)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="W11" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="W11" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I11="", "", ROUND(('3rd-Summary-Male'!I11+'3rd-Summary-Male'!J11)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X11" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C11="", "", ROUND(('4th-Summary-Male'!C11+'4th-Summary-Male'!D11)/2, 0))</f>
@@ -16764,9 +16768,9 @@
         <f aca="false">IF('2nd-Summary-Male'!I13="", "", ROUND(('2nd-Summary-Male'!I13+'2nd-Summary-Male'!J13)/2, 0))</f>
         <v>85</v>
       </c>
-      <c r="Q13" s="9" t="str">
+      <c r="Q13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!C13="", "", ROUND(('3rd-Summary-Male'!C13+'3rd-Summary-Male'!D13)/2, 0))</f>
-        <v/>
+        <v>77</v>
       </c>
       <c r="R13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!D13="", "", ROUND(('3rd-Summary-Male'!D13+'3rd-Summary-Male'!E13)/2, 0))</f>
@@ -16786,11 +16790,11 @@
       </c>
       <c r="V13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H13="", "", ROUND(('3rd-Summary-Male'!H13+'3rd-Summary-Male'!I13)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="W13" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="W13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I13="", "", ROUND(('3rd-Summary-Male'!I13+'3rd-Summary-Male'!J13)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X13" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C13="", "", ROUND(('4th-Summary-Male'!C13+'4th-Summary-Male'!D13)/2, 0))</f>
@@ -16830,9 +16834,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C22), "", CONCATENATE('Class-Infos'!C22, ", ", 'Class-Infos'!D22, " ", 'Class-Infos'!E22))</f>
         <v>ARROYO, AGA CEAZAR CAPALARAN</v>
       </c>
-      <c r="C14" s="8" t="str">
+      <c r="C14" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!C14="", "", ROUND(('1st-Summary-Male'!C14+'1st-Summary-Male'!D14)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="D14" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!D14="", "", ROUND(('1st-Summary-Male'!D14+'1st-Summary-Male'!E14)/2, 0))</f>
@@ -17124,7 +17128,7 @@
       </c>
       <c r="O16" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H16="", "", ROUND(('2nd-Summary-Male'!H16+'2nd-Summary-Male'!I16)/2, 0))</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P16" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!I16="", "", ROUND(('2nd-Summary-Male'!I16+'2nd-Summary-Male'!J16)/2, 0))</f>
@@ -17320,11 +17324,11 @@
       </c>
       <c r="C18" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!C18="", "", ROUND(('1st-Summary-Male'!C18+'1st-Summary-Male'!D18)/2, 0))</f>
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D18" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!D18="", "", ROUND(('1st-Summary-Male'!D18+'1st-Summary-Male'!E18)/2, 0))</f>
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E18" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!E18="", "", ROUND(('1st-Summary-Male'!E18+'1st-Summary-Male'!F18)/2, 0))</f>
@@ -17454,11 +17458,11 @@
       </c>
       <c r="F19" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!F19="", "", ROUND(('1st-Summary-Male'!F19+'1st-Summary-Male'!G19)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="G19" s="8" t="str">
+        <v>75</v>
+      </c>
+      <c r="G19" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!G19="", "", ROUND(('1st-Summary-Male'!G19+'1st-Summary-Male'!H19)/2, 0))</f>
-        <v/>
+        <v>72</v>
       </c>
       <c r="H19" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!H19="", "", ROUND(('1st-Summary-Male'!H19+'1st-Summary-Male'!I19)/2, 0))</f>
@@ -17482,23 +17486,23 @@
       </c>
       <c r="M19" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!F19="", "", ROUND(('2nd-Summary-Male'!F19+'2nd-Summary-Male'!G19)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="N19" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="N19" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!G19="", "", ROUND(('2nd-Summary-Male'!G19+'2nd-Summary-Male'!H19)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="O19" s="9" t="str">
+        <v>73</v>
+      </c>
+      <c r="O19" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!H19="", "", ROUND(('2nd-Summary-Male'!H19+'2nd-Summary-Male'!I19)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="P19" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Male'!I19="", "", ROUND(('2nd-Summary-Male'!I19+'2nd-Summary-Male'!J19)/2, 0))</f>
         <v>81</v>
       </c>
-      <c r="Q19" s="9" t="str">
+      <c r="Q19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!C19="", "", ROUND(('3rd-Summary-Male'!C19+'3rd-Summary-Male'!D19)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="R19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!D19="", "", ROUND(('3rd-Summary-Male'!D19+'3rd-Summary-Male'!E19)/2, 0))</f>
@@ -17510,19 +17514,19 @@
       </c>
       <c r="T19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F19="", "", ROUND(('3rd-Summary-Male'!F19+'3rd-Summary-Male'!G19)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="U19" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="U19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G19="", "", ROUND(('3rd-Summary-Male'!G19+'3rd-Summary-Male'!H19)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="V19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H19="", "", ROUND(('3rd-Summary-Male'!H19+'3rd-Summary-Male'!I19)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="W19" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="W19" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I19="", "", ROUND(('3rd-Summary-Male'!I19+'3rd-Summary-Male'!J19)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X19" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C19="", "", ROUND(('4th-Summary-Male'!C19+'4th-Summary-Male'!D19)/2, 0))</f>
@@ -17576,11 +17580,11 @@
       </c>
       <c r="F20" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!F20="", "", ROUND(('1st-Summary-Male'!F20+'1st-Summary-Male'!G20)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="G20" s="8" t="str">
+        <v>75</v>
+      </c>
+      <c r="G20" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!G20="", "", ROUND(('1st-Summary-Male'!G20+'1st-Summary-Male'!H20)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="H20" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!H20="", "", ROUND(('1st-Summary-Male'!H20+'1st-Summary-Male'!I20)/2, 0))</f>
@@ -17632,19 +17636,19 @@
       </c>
       <c r="T20" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F20="", "", ROUND(('3rd-Summary-Male'!F20+'3rd-Summary-Male'!G20)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U20" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U20" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G20="", "", ROUND(('3rd-Summary-Male'!G20+'3rd-Summary-Male'!H20)/2, 0))</f>
-        <v/>
+        <v>80</v>
       </c>
       <c r="V20" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H20="", "", ROUND(('3rd-Summary-Male'!H20+'3rd-Summary-Male'!I20)/2, 0))</f>
-        <v>41</v>
-      </c>
-      <c r="W20" s="9" t="str">
+        <v>79</v>
+      </c>
+      <c r="W20" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I20="", "", ROUND(('3rd-Summary-Male'!I20+'3rd-Summary-Male'!J20)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X20" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C20="", "", ROUND(('4th-Summary-Male'!C20+'4th-Summary-Male'!D20)/2, 0))</f>
@@ -17698,11 +17702,11 @@
       </c>
       <c r="F21" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!F21="", "", ROUND(('1st-Summary-Male'!F21+'1st-Summary-Male'!G21)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="G21" s="8" t="str">
+        <v>76</v>
+      </c>
+      <c r="G21" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!G21="", "", ROUND(('1st-Summary-Male'!G21+'1st-Summary-Male'!H21)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="H21" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!H21="", "", ROUND(('1st-Summary-Male'!H21+'1st-Summary-Male'!I21)/2, 0))</f>
@@ -17754,19 +17758,19 @@
       </c>
       <c r="T21" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F21="", "", ROUND(('3rd-Summary-Male'!F21+'3rd-Summary-Male'!G21)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U21" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U21" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G21="", "", ROUND(('3rd-Summary-Male'!G21+'3rd-Summary-Male'!H21)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="V21" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H21="", "", ROUND(('3rd-Summary-Male'!H21+'3rd-Summary-Male'!I21)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="W21" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="W21" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!I21="", "", ROUND(('3rd-Summary-Male'!I21+'3rd-Summary-Male'!J21)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X21" s="9" t="str">
         <f aca="false">IF('4th-Summary-Male'!C21="", "", ROUND(('4th-Summary-Male'!C21+'4th-Summary-Male'!D21)/2, 0))</f>
@@ -17806,9 +17810,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C30), "", CONCATENATE('Class-Infos'!C30, ", ", 'Class-Infos'!D30, " ", 'Class-Infos'!E30))</f>
         <v>BACLAAN, JOVART MATA</v>
       </c>
-      <c r="C22" s="8" t="str">
+      <c r="C22" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!C22="", "", ROUND(('1st-Summary-Male'!C22+'1st-Summary-Male'!D22)/2, 0))</f>
-        <v/>
+        <v>77</v>
       </c>
       <c r="D22" s="8" t="n">
         <f aca="false">IF('1st-Summary-Male'!D22="", "", ROUND(('1st-Summary-Male'!D22+'1st-Summary-Male'!E22)/2, 0))</f>
@@ -17876,11 +17880,11 @@
       </c>
       <c r="T22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!F22="", "", ROUND(('3rd-Summary-Male'!F22+'3rd-Summary-Male'!G22)/2, 0))</f>
-        <v>43</v>
-      </c>
-      <c r="U22" s="9" t="str">
+        <v>85</v>
+      </c>
+      <c r="U22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!G22="", "", ROUND(('3rd-Summary-Male'!G22+'3rd-Summary-Male'!H22)/2, 0))</f>
-        <v/>
+        <v>89</v>
       </c>
       <c r="V22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Male'!H22="", "", ROUND(('3rd-Summary-Male'!H22+'3rd-Summary-Male'!I22)/2, 0))</f>
@@ -20256,7 +20260,7 @@
   <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE37" activeCellId="1" sqref="M13:N13 AE37"/>
+      <selection pane="topLeft" activeCell="AE37" activeCellId="0" sqref="AE37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20295,94 +20299,94 @@
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20652,11 +20656,11 @@
       </c>
       <c r="F4" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F4="", "", ROUND(('1st-Summary-Female'!F4+'1st-Summary-Female'!G4)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="G4" s="9" t="str">
+        <v>79</v>
+      </c>
+      <c r="G4" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G4="", "", ROUND(('1st-Summary-Female'!G4+'1st-Summary-Female'!H4)/2, 0))</f>
-        <v/>
+        <v>82</v>
       </c>
       <c r="H4" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H4="", "", ROUND(('1st-Summary-Female'!H4+'1st-Summary-Female'!I4)/2, 0))</f>
@@ -21248,9 +21252,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C58), "", CONCATENATE('Class-Infos'!C58, ", ", 'Class-Infos'!D58, " ", 'Class-Infos'!E58))</f>
         <v>ALBIOLA, PRINCES DIANE FACTOR</v>
       </c>
-      <c r="C9" s="9" t="str">
+      <c r="C9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C9="", "", ROUND(('1st-Summary-Female'!C9+'1st-Summary-Female'!D9)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="D9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D9="", "", ROUND(('1st-Summary-Female'!D9+'1st-Summary-Female'!E9)/2, 0))</f>
@@ -21262,75 +21266,75 @@
       </c>
       <c r="F9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F9="", "", ROUND(('1st-Summary-Female'!F9+'1st-Summary-Female'!G9)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="G9" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="G9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G9="", "", ROUND(('1st-Summary-Female'!G9+'1st-Summary-Female'!H9)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="H9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H9="", "", ROUND(('1st-Summary-Female'!H9+'1st-Summary-Female'!I9)/2, 0))</f>
-        <v>36</v>
-      </c>
-      <c r="I9" s="9" t="str">
+        <v>71</v>
+      </c>
+      <c r="I9" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!I9="", "", ROUND(('1st-Summary-Female'!I9+'1st-Summary-Female'!J9)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="J9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!C9="", "", ROUND(('2nd-Summary-Female'!C9+'2nd-Summary-Female'!D9)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="K9" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="K9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!D9="", "", ROUND(('2nd-Summary-Female'!D9+'2nd-Summary-Female'!E9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="L9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="L9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!E9="", "", ROUND(('2nd-Summary-Female'!E9+'2nd-Summary-Female'!F9)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="M9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F9="", "", ROUND(('2nd-Summary-Female'!F9+'2nd-Summary-Female'!G9)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="N9" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="N9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G9="", "", ROUND(('2nd-Summary-Female'!G9+'2nd-Summary-Female'!H9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="O9" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="O9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!H9="", "", ROUND(('2nd-Summary-Female'!H9+'2nd-Summary-Female'!I9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="P9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="P9" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!I9="", "", ROUND(('2nd-Summary-Female'!I9+'2nd-Summary-Female'!J9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="Q9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!C9="", "", ROUND(('3rd-Summary-Female'!C9+'3rd-Summary-Female'!D9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="R9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="R9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D9="", "", ROUND(('3rd-Summary-Female'!D9+'3rd-Summary-Female'!E9)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="S9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="S9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E9="", "", ROUND(('3rd-Summary-Female'!E9+'3rd-Summary-Female'!F9)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="T9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F9="", "", ROUND(('3rd-Summary-Female'!F9+'3rd-Summary-Female'!G9)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U9" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G9="", "", ROUND(('3rd-Summary-Female'!G9+'3rd-Summary-Female'!H9)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="V9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H9="", "", ROUND(('3rd-Summary-Female'!H9+'3rd-Summary-Female'!I9)/2, 0))</f>
-        <v>35</v>
-      </c>
-      <c r="W9" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="W9" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!I9="", "", ROUND(('3rd-Summary-Female'!I9+'3rd-Summary-Female'!J9)/2, 0))</f>
-        <v/>
+        <v>70</v>
       </c>
       <c r="X9" s="9" t="str">
         <f aca="false">IF('4th-Summary-Female'!C9="", "", ROUND(('4th-Summary-Female'!C9+'4th-Summary-Female'!D9)/2, 0))</f>
@@ -21370,13 +21374,13 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C59), "", CONCATENATE('Class-Infos'!C59, ", ", 'Class-Infos'!D59, " ", 'Class-Infos'!E59))</f>
         <v>ALCANTARA, MICHAELLA JEN RODELAS</v>
       </c>
-      <c r="C10" s="9" t="str">
+      <c r="C10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C10="", "", ROUND(('1st-Summary-Female'!C10+'1st-Summary-Female'!D10)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="D10" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="D10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D10="", "", ROUND(('1st-Summary-Female'!D10+'1st-Summary-Female'!E10)/2, 0))</f>
-        <v/>
+        <v>72</v>
       </c>
       <c r="E10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!E10="", "", ROUND(('1st-Summary-Female'!E10+'1st-Summary-Female'!F10)/2, 0))</f>
@@ -21384,11 +21388,11 @@
       </c>
       <c r="F10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F10="", "", ROUND(('1st-Summary-Female'!F10+'1st-Summary-Female'!G10)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="G10" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="G10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G10="", "", ROUND(('1st-Summary-Female'!G10+'1st-Summary-Female'!H10)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="H10" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H10="", "", ROUND(('1st-Summary-Female'!H10+'1st-Summary-Female'!I10)/2, 0))</f>
@@ -21400,59 +21404,59 @@
       </c>
       <c r="J10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!C10="", "", ROUND(('2nd-Summary-Female'!C10+'2nd-Summary-Female'!D10)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="K10" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="K10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!D10="", "", ROUND(('2nd-Summary-Female'!D10+'2nd-Summary-Female'!E10)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="L10" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="L10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!E10="", "", ROUND(('2nd-Summary-Female'!E10+'2nd-Summary-Female'!F10)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="M10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F10="", "", ROUND(('2nd-Summary-Female'!F10+'2nd-Summary-Female'!G10)/2, 0))</f>
-        <v>40</v>
-      </c>
-      <c r="N10" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="N10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G10="", "", ROUND(('2nd-Summary-Female'!G10+'2nd-Summary-Female'!H10)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="O10" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="O10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!H10="", "", ROUND(('2nd-Summary-Female'!H10+'2nd-Summary-Female'!I10)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="P10" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!I10="", "", ROUND(('2nd-Summary-Female'!I10+'2nd-Summary-Female'!J10)/2, 0))</f>
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="Q10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!C10="", "", ROUND(('3rd-Summary-Female'!C10+'3rd-Summary-Female'!D10)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="R10" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="R10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D10="", "", ROUND(('3rd-Summary-Female'!D10+'3rd-Summary-Female'!E10)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="S10" s="9" t="str">
+        <v>70</v>
+      </c>
+      <c r="S10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E10="", "", ROUND(('3rd-Summary-Female'!E10+'3rd-Summary-Female'!F10)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="T10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F10="", "", ROUND(('3rd-Summary-Female'!F10+'3rd-Summary-Female'!G10)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U10" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="U10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G10="", "", ROUND(('3rd-Summary-Female'!G10+'3rd-Summary-Female'!H10)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="V10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H10="", "", ROUND(('3rd-Summary-Female'!H10+'3rd-Summary-Female'!I10)/2, 0))</f>
-        <v>35</v>
-      </c>
-      <c r="W10" s="9" t="str">
+        <v>73</v>
+      </c>
+      <c r="W10" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!I10="", "", ROUND(('3rd-Summary-Female'!I10+'3rd-Summary-Female'!J10)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="X10" s="9" t="str">
         <f aca="false">IF('4th-Summary-Female'!C10="", "", ROUND(('4th-Summary-Female'!C10+'4th-Summary-Female'!D10)/2, 0))</f>
@@ -21656,11 +21660,11 @@
       </c>
       <c r="M12" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F12="", "", ROUND(('2nd-Summary-Female'!F12+'2nd-Summary-Female'!G12)/2, 0))</f>
-        <v>44</v>
-      </c>
-      <c r="N12" s="9" t="str">
+        <v>81</v>
+      </c>
+      <c r="N12" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G12="", "", ROUND(('2nd-Summary-Female'!G12+'2nd-Summary-Female'!H12)/2, 0))</f>
-        <v/>
+        <v>82</v>
       </c>
       <c r="O12" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!H12="", "", ROUND(('2nd-Summary-Female'!H12+'2nd-Summary-Female'!I12)/2, 0))</f>
@@ -21736,9 +21740,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C62), "", CONCATENATE('Class-Infos'!C62, ", ", 'Class-Infos'!D62, " ", 'Class-Infos'!E62))</f>
         <v>AMBULO, PRINCESS ANNE BASILIO</v>
       </c>
-      <c r="C13" s="9" t="str">
+      <c r="C13" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C13="", "", ROUND(('1st-Summary-Female'!C13+'1st-Summary-Female'!D13)/2, 0))</f>
-        <v/>
+        <v>77</v>
       </c>
       <c r="D13" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D13="", "", ROUND(('1st-Summary-Female'!D13+'1st-Summary-Female'!E13)/2, 0))</f>
@@ -21750,11 +21754,11 @@
       </c>
       <c r="F13" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F13="", "", ROUND(('1st-Summary-Female'!F13+'1st-Summary-Female'!G13)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="G13" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="G13" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G13="", "", ROUND(('1st-Summary-Female'!G13+'1st-Summary-Female'!H13)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="H13" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H13="", "", ROUND(('1st-Summary-Female'!H13+'1st-Summary-Female'!I13)/2, 0))</f>
@@ -21778,15 +21782,15 @@
       </c>
       <c r="M13" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F13="", "", ROUND(('2nd-Summary-Female'!F13+'2nd-Summary-Female'!G13)/2, 0))</f>
-        <v>40</v>
-      </c>
-      <c r="N13" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="N13" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G13="", "", ROUND(('2nd-Summary-Female'!G13+'2nd-Summary-Female'!H13)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="O13" s="9" t="str">
+        <v>73</v>
+      </c>
+      <c r="O13" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!H13="", "", ROUND(('2nd-Summary-Female'!H13+'2nd-Summary-Female'!I13)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="P13" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!I13="", "", ROUND(('2nd-Summary-Female'!I13+'2nd-Summary-Female'!J13)/2, 0))</f>
@@ -21798,19 +21802,19 @@
       </c>
       <c r="R13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D13="", "", ROUND(('3rd-Summary-Female'!D13+'3rd-Summary-Female'!E13)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="S13" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="S13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E13="", "", ROUND(('3rd-Summary-Female'!E13+'3rd-Summary-Female'!F13)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="T13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F13="", "", ROUND(('3rd-Summary-Female'!F13+'3rd-Summary-Female'!G13)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U13" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="U13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G13="", "", ROUND(('3rd-Summary-Female'!G13+'3rd-Summary-Female'!H13)/2, 0))</f>
-        <v/>
+        <v>72</v>
       </c>
       <c r="V13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H13="", "", ROUND(('3rd-Summary-Female'!H13+'3rd-Summary-Female'!I13)/2, 0))</f>
@@ -21818,7 +21822,7 @@
       </c>
       <c r="W13" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!I13="", "", ROUND(('3rd-Summary-Female'!I13+'3rd-Summary-Female'!J13)/2, 0))</f>
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="X13" s="9" t="str">
         <f aca="false">IF('4th-Summary-Female'!C13="", "", ROUND(('4th-Summary-Female'!C13+'4th-Summary-Female'!D13)/2, 0))</f>
@@ -22050,19 +22054,19 @@
       </c>
       <c r="T15" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F15="", "", ROUND(('3rd-Summary-Female'!F15+'3rd-Summary-Female'!G15)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U15" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="U15" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G15="", "", ROUND(('3rd-Summary-Female'!G15+'3rd-Summary-Female'!H15)/2, 0))</f>
-        <v/>
+        <v>83</v>
       </c>
       <c r="V15" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H15="", "", ROUND(('3rd-Summary-Female'!H15+'3rd-Summary-Female'!I15)/2, 0))</f>
-        <v>43</v>
-      </c>
-      <c r="W15" s="9" t="str">
+        <v>80</v>
+      </c>
+      <c r="W15" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!I15="", "", ROUND(('3rd-Summary-Female'!I15+'3rd-Summary-Female'!J15)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="X15" s="9" t="str">
         <f aca="false">IF('4th-Summary-Female'!C15="", "", ROUND(('4th-Summary-Female'!C15+'4th-Summary-Female'!D15)/2, 0))</f>
@@ -22102,9 +22106,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C65), "", CONCATENATE('Class-Infos'!C65, ", ", 'Class-Infos'!D65, " ", 'Class-Infos'!E65))</f>
         <v>ARCANGEL, MIKA ELLA CAMIGLA</v>
       </c>
-      <c r="C16" s="9" t="str">
+      <c r="C16" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C16="", "", ROUND(('1st-Summary-Female'!C16+'1st-Summary-Female'!D16)/2, 0))</f>
-        <v/>
+        <v>76</v>
       </c>
       <c r="D16" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D16="", "", ROUND(('1st-Summary-Female'!D16+'1st-Summary-Female'!E16)/2, 0))</f>
@@ -22172,11 +22176,11 @@
       </c>
       <c r="T16" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F16="", "", ROUND(('3rd-Summary-Female'!F16+'3rd-Summary-Female'!G16)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="U16" s="9" t="str">
+        <v>78</v>
+      </c>
+      <c r="U16" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G16="", "", ROUND(('3rd-Summary-Female'!G16+'3rd-Summary-Female'!H16)/2, 0))</f>
-        <v/>
+        <v>81</v>
       </c>
       <c r="V16" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H16="", "", ROUND(('3rd-Summary-Female'!H16+'3rd-Summary-Female'!I16)/2, 0))</f>
@@ -22360,11 +22364,11 @@
       </c>
       <c r="F18" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F18="", "", ROUND(('1st-Summary-Female'!F18+'1st-Summary-Female'!G18)/2, 0))</f>
-        <v>41</v>
-      </c>
-      <c r="G18" s="9" t="str">
+        <v>79</v>
+      </c>
+      <c r="G18" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G18="", "", ROUND(('1st-Summary-Female'!G18+'1st-Summary-Female'!H18)/2, 0))</f>
-        <v/>
+        <v>76</v>
       </c>
       <c r="H18" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H18="", "", ROUND(('1st-Summary-Female'!H18+'1st-Summary-Female'!I18)/2, 0))</f>
@@ -22468,9 +22472,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C68), "", CONCATENATE('Class-Infos'!C68, ", ", 'Class-Infos'!D68, " ", 'Class-Infos'!E68))</f>
         <v>AVECILLA, JEAN RAIZHEN SALAZAR</v>
       </c>
-      <c r="C19" s="9" t="str">
+      <c r="C19" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C19="", "", ROUND(('1st-Summary-Female'!C19+'1st-Summary-Female'!D19)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="D19" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D19="", "", ROUND(('1st-Summary-Female'!D19+'1st-Summary-Female'!E19)/2, 0))</f>
@@ -22620,11 +22624,11 @@
       </c>
       <c r="J20" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!C20="", "", ROUND(('2nd-Summary-Female'!C20+'2nd-Summary-Female'!D20)/2, 0))</f>
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="K20" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!D20="", "", ROUND(('2nd-Summary-Female'!D20+'2nd-Summary-Female'!E20)/2, 0))</f>
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="L20" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!E20="", "", ROUND(('2nd-Summary-Female'!E20+'2nd-Summary-Female'!F20)/2, 0))</f>
@@ -22832,7 +22836,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C22="", "", ROUND(('1st-Summary-Female'!C22+'1st-Summary-Female'!D22)/2, 0))</f>
@@ -22896,11 +22900,11 @@
       </c>
       <c r="R22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D22="", "", ROUND(('3rd-Summary-Female'!D22+'3rd-Summary-Female'!E22)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="S22" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="S22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E22="", "", ROUND(('3rd-Summary-Female'!E22+'3rd-Summary-Female'!F22)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="T22" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F22="", "", ROUND(('3rd-Summary-Female'!F22+'3rd-Summary-Female'!G22)/2, 0))</f>
@@ -22986,11 +22990,11 @@
       </c>
       <c r="J23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!C23="", "", ROUND(('2nd-Summary-Female'!C23+'2nd-Summary-Female'!D23)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="K23" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="K23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!D23="", "", ROUND(('2nd-Summary-Female'!D23+'2nd-Summary-Female'!E23)/2, 0))</f>
-        <v/>
+        <v>74</v>
       </c>
       <c r="L23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!E23="", "", ROUND(('2nd-Summary-Female'!E23+'2nd-Summary-Female'!F23)/2, 0))</f>
@@ -22998,11 +23002,11 @@
       </c>
       <c r="M23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F23="", "", ROUND(('2nd-Summary-Female'!F23+'2nd-Summary-Female'!G23)/2, 0))</f>
-        <v>39</v>
-      </c>
-      <c r="N23" s="9" t="str">
+        <v>76</v>
+      </c>
+      <c r="N23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G23="", "", ROUND(('2nd-Summary-Female'!G23+'2nd-Summary-Female'!H23)/2, 0))</f>
-        <v/>
+        <v>79</v>
       </c>
       <c r="O23" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!H23="", "", ROUND(('2nd-Summary-Female'!H23+'2nd-Summary-Female'!I23)/2, 0))</f>
@@ -23014,23 +23018,23 @@
       </c>
       <c r="Q23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!C23="", "", ROUND(('3rd-Summary-Female'!C23+'3rd-Summary-Female'!D23)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="R23" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="R23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D23="", "", ROUND(('3rd-Summary-Female'!D23+'3rd-Summary-Female'!E23)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="S23" s="9" t="str">
+        <v>74</v>
+      </c>
+      <c r="S23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E23="", "", ROUND(('3rd-Summary-Female'!E23+'3rd-Summary-Female'!F23)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="T23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F23="", "", ROUND(('3rd-Summary-Female'!F23+'3rd-Summary-Female'!G23)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="U23" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="U23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G23="", "", ROUND(('3rd-Summary-Female'!G23+'3rd-Summary-Female'!H23)/2, 0))</f>
-        <v/>
+        <v>79</v>
       </c>
       <c r="V23" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H23="", "", ROUND(('3rd-Summary-Female'!H23+'3rd-Summary-Female'!I23)/2, 0))</f>
@@ -23200,25 +23204,25 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C74), "", CONCATENATE('Class-Infos'!C74, ", ", 'Class-Infos'!D74, " ", 'Class-Infos'!E74))</f>
         <v>SARDIDO, GEMMA LEE SORIANO</v>
       </c>
-      <c r="C25" s="9" t="str">
+      <c r="C25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!C25="", "", ROUND(('1st-Summary-Female'!C25+'1st-Summary-Female'!D25)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="D25" s="9" t="str">
+        <v>75</v>
+      </c>
+      <c r="D25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!D25="", "", ROUND(('1st-Summary-Female'!D25+'1st-Summary-Female'!E25)/2, 0))</f>
-        <v/>
+        <v>75</v>
       </c>
       <c r="E25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!E25="", "", ROUND(('1st-Summary-Female'!E25+'1st-Summary-Female'!F25)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="F25" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="F25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!F25="", "", ROUND(('1st-Summary-Female'!F25+'1st-Summary-Female'!G25)/2, 0))</f>
-        <v/>
-      </c>
-      <c r="G25" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="G25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!G25="", "", ROUND(('1st-Summary-Female'!G25+'1st-Summary-Female'!H25)/2, 0))</f>
-        <v/>
+        <v>72</v>
       </c>
       <c r="H25" s="9" t="n">
         <f aca="false">IF('1st-Summary-Female'!H25="", "", ROUND(('1st-Summary-Female'!H25+'1st-Summary-Female'!I25)/2, 0))</f>
@@ -23238,11 +23242,11 @@
       </c>
       <c r="L25" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!E25="", "", ROUND(('2nd-Summary-Female'!E25+'2nd-Summary-Female'!F25)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="M25" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="M25" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!F25="", "", ROUND(('2nd-Summary-Female'!F25+'2nd-Summary-Female'!G25)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="N25" s="9" t="n">
         <f aca="false">IF('2nd-Summary-Female'!G25="", "", ROUND(('2nd-Summary-Female'!G25+'2nd-Summary-Female'!H25)/2, 0))</f>
@@ -23262,27 +23266,27 @@
       </c>
       <c r="R25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!D25="", "", ROUND(('3rd-Summary-Female'!D25+'3rd-Summary-Female'!E25)/2, 0))</f>
-        <v>38</v>
-      </c>
-      <c r="S25" s="9" t="str">
+        <v>73</v>
+      </c>
+      <c r="S25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!E25="", "", ROUND(('3rd-Summary-Female'!E25+'3rd-Summary-Female'!F25)/2, 0))</f>
-        <v/>
+        <v>72</v>
       </c>
       <c r="T25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!F25="", "", ROUND(('3rd-Summary-Female'!F25+'3rd-Summary-Female'!G25)/2, 0))</f>
-        <v>37</v>
-      </c>
-      <c r="U25" s="9" t="str">
+        <v>72</v>
+      </c>
+      <c r="U25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!G25="", "", ROUND(('3rd-Summary-Female'!G25+'3rd-Summary-Female'!H25)/2, 0))</f>
-        <v/>
+        <v>77</v>
       </c>
       <c r="V25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!H25="", "", ROUND(('3rd-Summary-Female'!H25+'3rd-Summary-Female'!I25)/2, 0))</f>
-        <v>42</v>
-      </c>
-      <c r="W25" s="9" t="str">
+        <v>77</v>
+      </c>
+      <c r="W25" s="9" t="n">
         <f aca="false">IF('3rd-Summary-Female'!I25="", "", ROUND(('3rd-Summary-Female'!I25+'3rd-Summary-Female'!J25)/2, 0))</f>
-        <v/>
+        <v>73</v>
       </c>
       <c r="X25" s="9" t="str">
         <f aca="false">IF('4th-Summary-Female'!C25="", "", ROUND(('4th-Summary-Female'!C25+'4th-Summary-Female'!D25)/2, 0))</f>
@@ -25284,7 +25288,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="M13:N13 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25297,7 +25301,7 @@
         <v>75</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25308,7 +25312,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25319,7 +25323,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25330,7 +25334,7 @@
         <v>99</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -25356,7 +25360,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="1" sqref="M13:N13 B42"/>
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25372,16 +25376,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>151</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
@@ -25393,16 +25397,16 @@
         <v>11</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27273,7 +27277,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="M13:N13 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27289,16 +27293,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>151</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>2</v>
@@ -27310,16 +27314,16 @@
         <v>11</v>
       </c>
       <c r="H1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28249,7 +28253,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="7" t="n">
         <f aca="false">IF(ISBLANK('Class-Infos'!G71), "", 'Class-Infos'!G71)</f>
@@ -29190,7 +29194,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O16" activeCellId="1" sqref="M13:N13 O16"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29202,46 +29206,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29483,6 +29487,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C15), "", CONCATENATE('Class-Infos'!C15, ", ", 'Class-Infos'!D15, " ", 'Class-Infos'!E15))</f>
         <v>ALEJANDRO, MARK AGBUYA</v>
       </c>
+      <c r="C7" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D7" s="8" t="n">
         <v>75</v>
       </c>
@@ -29676,6 +29683,9 @@
       <c r="F11" s="8" t="n">
         <v>76</v>
       </c>
+      <c r="G11" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H11" s="8" t="n">
         <v>75</v>
       </c>
@@ -29799,6 +29809,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C22), "", CONCATENATE('Class-Infos'!C22, ", ", 'Class-Infos'!D22, " ", 'Class-Infos'!E22))</f>
         <v>ARROYO, AGA CEAZAR CAPALARAN</v>
       </c>
+      <c r="C14" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D14" s="8" t="n">
         <v>75</v>
       </c>
@@ -29984,7 +29997,7 @@
         <v>75</v>
       </c>
       <c r="D18" s="8" t="n">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>74</v>
@@ -30038,6 +30051,9 @@
       <c r="F19" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G19" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H19" s="8" t="n">
         <v>70</v>
       </c>
@@ -30081,6 +30097,9 @@
       <c r="F20" s="8" t="n">
         <v>76</v>
       </c>
+      <c r="G20" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H20" s="8" t="n">
         <v>75</v>
       </c>
@@ -30124,6 +30143,9 @@
       <c r="F21" s="8" t="n">
         <v>77</v>
       </c>
+      <c r="G21" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H21" s="8" t="n">
         <v>75</v>
       </c>
@@ -30154,6 +30176,9 @@
       <c r="B22" s="7" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C30), "", CONCATENATE('Class-Infos'!C30, ", ", 'Class-Infos'!D30, " ", 'Class-Infos'!E30))</f>
         <v>BACLAAN, JOVART MATA</v>
+      </c>
+      <c r="C22" s="8" t="n">
+        <v>73</v>
       </c>
       <c r="D22" s="8" t="n">
         <v>81</v>
@@ -30645,8 +30670,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L26" activeCellId="1" sqref="M13:N13 L26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30658,46 +30683,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -30813,6 +30838,9 @@
       <c r="F4" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="G4" s="8" t="n">
+        <v>80</v>
+      </c>
       <c r="H4" s="8" t="n">
         <v>83</v>
       </c>
@@ -31028,6 +31056,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C58), "", CONCATENATE('Class-Infos'!C58, ", ", 'Class-Infos'!D58, " ", 'Class-Infos'!E58))</f>
         <v>ALBIOLA, PRINCES DIANE FACTOR</v>
       </c>
+      <c r="C9" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D9" s="8" t="n">
         <v>76</v>
       </c>
@@ -31037,8 +31068,14 @@
       <c r="F9" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G9" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H9" s="8" t="n">
         <v>72</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>70</v>
       </c>
       <c r="J9" s="8" t="n">
         <v>75</v>
@@ -31065,11 +31102,20 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C59), "", CONCATENATE('Class-Infos'!C59, ", ", 'Class-Infos'!D59, " ", 'Class-Infos'!E59))</f>
         <v>ALCANTARA, MICHAELLA JEN RODELAS</v>
       </c>
+      <c r="C10" s="8" t="n">
+        <v>73</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="E10" s="8" t="n">
         <v>74</v>
       </c>
       <c r="F10" s="8" t="n">
         <v>77</v>
+      </c>
+      <c r="G10" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="H10" s="8" t="n">
         <v>75</v>
@@ -31194,6 +31240,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C62), "", CONCATENATE('Class-Infos'!C62, ", ", 'Class-Infos'!D62, " ", 'Class-Infos'!E62))</f>
         <v>AMBULO, PRINCESS ANNE BASILIO</v>
       </c>
+      <c r="C13" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D13" s="8" t="n">
         <v>81</v>
       </c>
@@ -31202,6 +31251,9 @@
       </c>
       <c r="F13" s="8" t="n">
         <v>78</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>75</v>
@@ -31326,6 +31378,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C65), "", CONCATENATE('Class-Infos'!C65, ", ", 'Class-Infos'!D65, " ", 'Class-Infos'!E65))</f>
         <v>ARCANGEL, MIKA ELLA CAMIGLA</v>
       </c>
+      <c r="C16" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D16" s="8" t="n">
         <v>79</v>
       </c>
@@ -31427,6 +31482,9 @@
       <c r="F18" s="8" t="n">
         <v>82</v>
       </c>
+      <c r="G18" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H18" s="8" t="n">
         <v>76</v>
       </c>
@@ -31458,6 +31516,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C68), "", CONCATENATE('Class-Infos'!C68, ", ", 'Class-Infos'!D68, " ", 'Class-Infos'!E68))</f>
         <v>AVECILLA, JEAN RAIZHEN SALAZAR</v>
       </c>
+      <c r="C19" s="8" t="n">
+        <v>73</v>
+      </c>
       <c r="D19" s="8" t="n">
         <v>77</v>
       </c>
@@ -31591,7 +31652,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="8" t="n">
         <v>75</v>
@@ -31731,7 +31792,19 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C74), "", CONCATENATE('Class-Infos'!C74, ", ", 'Class-Infos'!D74, " ", 'Class-Infos'!E74))</f>
         <v>SARDIDO, GEMMA LEE SORIANO</v>
       </c>
+      <c r="C25" s="8" t="n">
+        <v>73</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>76</v>
+      </c>
       <c r="E25" s="8" t="n">
+        <v>74</v>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="G25" s="8" t="n">
         <v>74</v>
       </c>
       <c r="H25" s="8" t="n">
@@ -31934,8 +32007,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="1" sqref="M13:N13 N12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31947,46 +32020,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32148,11 +32221,29 @@
       <c r="F5" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="G5" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H5" s="8" t="n">
         <v>73</v>
       </c>
       <c r="I5" s="8" t="n">
         <v>76</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="N5" s="8" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32222,10 +32313,28 @@
       <c r="F7" s="8" t="n">
         <v>76</v>
       </c>
+      <c r="G7" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H7" s="8" t="n">
         <v>81</v>
       </c>
       <c r="I7" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="N7" s="8" t="n">
         <v>75</v>
       </c>
     </row>
@@ -32250,6 +32359,9 @@
       <c r="F8" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="G8" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H8" s="8" t="n">
         <v>86</v>
       </c>
@@ -32339,6 +32451,9 @@
       <c r="F10" s="8" t="n">
         <v>80</v>
       </c>
+      <c r="G10" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H10" s="8" t="n">
         <v>86</v>
       </c>
@@ -32382,6 +32497,9 @@
       <c r="F11" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="G11" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H11" s="8" t="n">
         <v>87</v>
       </c>
@@ -32613,7 +32731,7 @@
         <v>83</v>
       </c>
       <c r="H16" s="8" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I16" s="8" t="n">
         <v>78</v>
@@ -32746,6 +32864,12 @@
       </c>
       <c r="F19" s="8" t="n">
         <v>76</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="H19" s="8" t="n">
+        <v>70</v>
       </c>
       <c r="I19" s="8" t="n">
         <v>76</v>
@@ -33100,8 +33224,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="1" sqref="M13:N13 M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33113,46 +33237,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33489,8 +33613,38 @@
       <c r="C9" s="8" t="n">
         <v>74</v>
       </c>
+      <c r="D9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="F9" s="8" t="n">
         <v>76</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>74</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="K9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="L9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33505,11 +33659,38 @@
       <c r="C10" s="8" t="n">
         <v>74</v>
       </c>
+      <c r="D10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="F10" s="8" t="n">
         <v>79</v>
       </c>
+      <c r="G10" s="8" t="n">
+        <v>74</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="I10" s="8" t="n">
         <v>75</v>
+      </c>
+      <c r="J10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="K10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="L10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33579,6 +33760,9 @@
       <c r="F12" s="8" t="n">
         <v>87</v>
       </c>
+      <c r="G12" s="8" t="n">
+        <v>75</v>
+      </c>
       <c r="H12" s="8" t="n">
         <v>88</v>
       </c>
@@ -33622,6 +33806,12 @@
       <c r="F13" s="8" t="n">
         <v>79</v>
       </c>
+      <c r="G13" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="I13" s="8" t="n">
         <v>75</v>
       </c>
@@ -33930,7 +34120,7 @@
         <v>92</v>
       </c>
       <c r="D20" s="8" t="n">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>82</v>
@@ -34016,7 +34206,7 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="8" t="n">
         <v>75</v>
@@ -34067,11 +34257,17 @@
       <c r="C23" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="D23" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="E23" s="8" t="n">
         <v>74</v>
       </c>
       <c r="F23" s="8" t="n">
         <v>77</v>
+      </c>
+      <c r="G23" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="H23" s="8" t="n">
         <v>82</v>
@@ -34158,6 +34354,9 @@
       </c>
       <c r="E25" s="8" t="n">
         <v>74</v>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>70</v>
       </c>
       <c r="G25" s="8" t="n">
         <v>75</v>
@@ -34362,8 +34561,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="1" sqref="M13:N13 M5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34375,46 +34574,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34570,11 +34769,20 @@
       <c r="D5" s="8" t="n">
         <v>80</v>
       </c>
+      <c r="E5" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="F5" s="8" t="n">
         <v>75</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>76</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>83</v>
+      </c>
+      <c r="I5" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J5" s="8" t="n">
         <v>75</v>
@@ -34659,8 +34867,14 @@
       <c r="F7" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G7" s="8" t="n">
+        <v>76</v>
+      </c>
       <c r="H7" s="8" t="n">
         <v>84</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J7" s="8" t="n">
         <v>75</v>
@@ -34699,8 +34913,14 @@
       <c r="F8" s="8" t="n">
         <v>80</v>
       </c>
+      <c r="G8" s="8" t="n">
+        <v>78</v>
+      </c>
       <c r="H8" s="8" t="n">
         <v>84</v>
+      </c>
+      <c r="I8" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J8" s="8" t="n">
         <v>75</v>
@@ -34785,8 +35005,14 @@
       <c r="F10" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="G10" s="8" t="n">
+        <v>78</v>
+      </c>
       <c r="H10" s="8" t="n">
         <v>90</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J10" s="8" t="n">
         <v>75</v>
@@ -34825,8 +35051,14 @@
       <c r="F11" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G11" s="8" t="n">
+        <v>76</v>
+      </c>
       <c r="H11" s="8" t="n">
         <v>73</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J11" s="8" t="n">
         <v>75</v>
@@ -34899,6 +35131,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C21), "", CONCATENATE('Class-Infos'!C21, ", ", 'Class-Infos'!D21, " ", 'Class-Infos'!E21))</f>
         <v>ARESGADO, CHRISTIAN MACKY MANUEL</v>
       </c>
+      <c r="C13" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="D13" s="8" t="n">
         <v>79</v>
       </c>
@@ -34912,6 +35147,9 @@
         <v>80</v>
       </c>
       <c r="H13" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="I13" s="8" t="n">
         <v>75</v>
       </c>
       <c r="J13" s="8" t="n">
@@ -35169,6 +35407,9 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C27), "", CONCATENATE('Class-Infos'!C27, ", ", 'Class-Infos'!D27, " ", 'Class-Infos'!E27))</f>
         <v>AYOP, WESLEY MICHEN BALBUENA</v>
       </c>
+      <c r="C19" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="D19" s="8" t="n">
         <v>76</v>
       </c>
@@ -35178,8 +35419,14 @@
       <c r="F19" s="8" t="n">
         <v>74</v>
       </c>
+      <c r="G19" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="H19" s="8" t="n">
         <v>73</v>
+      </c>
+      <c r="I19" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="J19" s="8" t="n">
         <v>75</v>
@@ -35218,8 +35465,14 @@
       <c r="F20" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G20" s="8" t="n">
+        <v>77</v>
+      </c>
       <c r="H20" s="8" t="n">
         <v>82</v>
+      </c>
+      <c r="I20" s="8" t="n">
+        <v>75</v>
       </c>
       <c r="J20" s="8" t="n">
         <v>75</v>
@@ -35258,8 +35511,14 @@
       <c r="F21" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G21" s="8" t="n">
+        <v>76</v>
+      </c>
       <c r="H21" s="8" t="n">
         <v>73</v>
+      </c>
+      <c r="I21" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="J21" s="8" t="n">
         <v>75</v>
@@ -35296,6 +35555,9 @@
         <v>86</v>
       </c>
       <c r="F22" s="8" t="n">
+        <v>85</v>
+      </c>
+      <c r="G22" s="8" t="n">
         <v>85</v>
       </c>
       <c r="H22" s="8" t="n">
@@ -35516,8 +35778,8 @@
   </sheetPr>
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13:N13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35529,46 +35791,46 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35902,10 +36164,40 @@
         <f aca="false">IF(ISBLANK('Class-Infos'!C58), "", CONCATENATE('Class-Infos'!C58, ", ", 'Class-Infos'!D58, " ", 'Class-Infos'!E58))</f>
         <v>ALBIOLA, PRINCES DIANE FACTOR</v>
       </c>
+      <c r="C9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="F9" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G9" s="8" t="n">
+        <v>77</v>
+      </c>
       <c r="H9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="K9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="L9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="M9" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="N9" s="8" t="n">
         <v>70</v>
       </c>
     </row>
@@ -35919,12 +36211,39 @@
         <v>ALCANTARA, MICHAELLA JEN RODELAS</v>
       </c>
       <c r="C10" s="8" t="n">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="D10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>70</v>
       </c>
       <c r="F10" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G10" s="8" t="n">
+        <v>77</v>
+      </c>
       <c r="H10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="I10" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="J10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="K10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="L10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="M10" s="8" t="n">
+        <v>70</v>
+      </c>
+      <c r="N10" s="8" t="n">
         <v>70</v>
       </c>
     </row>
@@ -36035,14 +36354,35 @@
       <c r="D13" s="8" t="n">
         <v>78</v>
       </c>
+      <c r="E13" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="F13" s="8" t="n">
         <v>75</v>
+      </c>
+      <c r="G13" s="8" t="n">
+        <v>73</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>70</v>
       </c>
       <c r="I13" s="8" t="n">
         <v>75</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36112,8 +36452,14 @@
       <c r="F15" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="G15" s="8" t="n">
+        <v>79</v>
+      </c>
       <c r="H15" s="8" t="n">
         <v>86</v>
+      </c>
+      <c r="I15" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="J15" s="8" t="n">
         <v>75</v>
@@ -36152,6 +36498,9 @@
       <c r="F16" s="8" t="n">
         <v>77</v>
       </c>
+      <c r="G16" s="8" t="n">
+        <v>78</v>
+      </c>
       <c r="H16" s="8" t="n">
         <v>83</v>
       </c>
@@ -36411,13 +36760,16 @@
       </c>
       <c r="B22" s="0" t="str">
         <f aca="false">IF(ISBLANK('Class-Infos'!C71), "", CONCATENATE('Class-Infos'!C71, ", ", 'Class-Infos'!D71, " ", 'Class-Infos'!E71))</f>
-        <v>AZUCENAS, JURIELYN VILLAGANAS</v>
+        <v>AZUCENAS, JURIELYN </v>
       </c>
       <c r="C22" s="8" t="n">
         <v>76</v>
       </c>
       <c r="D22" s="8" t="n">
         <v>77</v>
+      </c>
+      <c r="E22" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="F22" s="8" t="n">
         <v>75</v>
@@ -36459,7 +36811,16 @@
       <c r="C23" s="8" t="n">
         <v>75</v>
       </c>
+      <c r="D23" s="8" t="n">
+        <v>74</v>
+      </c>
+      <c r="E23" s="8" t="n">
+        <v>74</v>
+      </c>
       <c r="F23" s="8" t="n">
+        <v>75</v>
+      </c>
+      <c r="G23" s="8" t="n">
         <v>75</v>
       </c>
       <c r="H23" s="8" t="n">
@@ -36545,11 +36906,20 @@
       <c r="D25" s="8" t="n">
         <v>76</v>
       </c>
+      <c r="E25" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="F25" s="8" t="n">
         <v>74</v>
       </c>
+      <c r="G25" s="8" t="n">
+        <v>70</v>
+      </c>
       <c r="H25" s="8" t="n">
         <v>84</v>
+      </c>
+      <c r="I25" s="8" t="n">
+        <v>70</v>
       </c>
       <c r="J25" s="8" t="n">
         <v>75</v>

</xml_diff>